<commit_message>
Added support for Pnuemo 65+
</commit_message>
<xml_diff>
--- a/schedules/Pneumo.xlsx
+++ b/schedules/Pneumo.xlsx
@@ -10,21 +10,22 @@
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="389"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Schedules" sheetId="1" r:id="rId1"/>
     <sheet name="XML" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Excel_BuiltIn_Print_Area_1_1">Schedules!$A$1:$L$144</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Schedules!$A$1:$L$181</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area_1_1">Schedules!$A$1:$L$149</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Schedules!$A$1:$L$188</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="76">
   <si>
     <t>Forecast Series Name</t>
   </si>
@@ -246,6 +247,12 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>Indication End</t>
+  </si>
+  <si>
+    <t>19 years</t>
   </si>
 </sst>
 </file>
@@ -465,7 +472,13 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -475,15 +488,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -503,6 +507,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -918,9 +925,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K180"/>
+  <dimension ref="B1:K187"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="C180" sqref="C180"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -947,13 +957,13 @@
       <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
@@ -1034,11 +1044,11 @@
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="6" t="s">
@@ -1094,12 +1104,12 @@
       <c r="F60" s="14"/>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B61" s="25" t="s">
+      <c r="B61" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C61" s="25"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="25"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="37"/>
+      <c r="E61" s="37"/>
       <c r="F61" s="14"/>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.2">
@@ -1174,956 +1184,958 @@
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B68" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C68" s="18"/>
-      <c r="D68" s="9" t="s">
-        <v>56</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D68" s="9"/>
       <c r="E68" s="9"/>
       <c r="F68" s="14"/>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B69" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C69" s="18"/>
-      <c r="D69" s="9"/>
+      <c r="D69" s="9" t="s">
+        <v>56</v>
+      </c>
       <c r="E69" s="9"/>
       <c r="F69" s="14"/>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B70" s="25" t="s">
+      <c r="B70" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C70" s="18"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="14"/>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B71" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="C70" s="25"/>
-      <c r="D70" s="25"/>
-      <c r="F70" s="14"/>
-    </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B71" s="6" t="s">
+      <c r="C71" s="37"/>
+      <c r="D71" s="37"/>
+      <c r="F71" s="14"/>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B72" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C71" s="6" t="s">
+      <c r="C72" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D71" s="6" t="s">
+      <c r="D72" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E71" s="6" t="s">
+      <c r="E72" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F71" s="26" t="s">
+      <c r="F72" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="G71" s="27"/>
-      <c r="H71" s="27"/>
-      <c r="I71" s="27"/>
-      <c r="J71" s="27"/>
-      <c r="K71" s="28"/>
-    </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B72" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C72" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D72" s="9"/>
-      <c r="E72" s="9"/>
-      <c r="F72" s="29"/>
-      <c r="G72" s="30"/>
-      <c r="H72" s="30"/>
-      <c r="I72" s="30"/>
-      <c r="J72" s="30"/>
-      <c r="K72" s="31"/>
+      <c r="G72" s="29"/>
+      <c r="H72" s="29"/>
+      <c r="I72" s="29"/>
+      <c r="J72" s="29"/>
+      <c r="K72" s="30"/>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B73" s="9" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="D73" s="9"/>
       <c r="E73" s="9"/>
-      <c r="F73" s="32" t="s">
+      <c r="F73" s="25"/>
+      <c r="G73" s="26"/>
+      <c r="H73" s="26"/>
+      <c r="I73" s="26"/>
+      <c r="J73" s="26"/>
+      <c r="K73" s="27"/>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B74" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="G73" s="33"/>
-      <c r="H73" s="33"/>
-      <c r="I73" s="33"/>
-      <c r="J73" s="33"/>
-      <c r="K73" s="34"/>
-    </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B74" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C74" s="9">
-        <v>1</v>
-      </c>
-      <c r="F74" s="14" t="s">
-        <v>62</v>
-      </c>
+      <c r="G74" s="32"/>
+      <c r="H74" s="32"/>
+      <c r="I74" s="32"/>
+      <c r="J74" s="32"/>
+      <c r="K74" s="33"/>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B75" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C75" s="9">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B77" s="5" t="s">
+      <c r="F75" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B76" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C76" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B78" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C78" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D77" s="14"/>
-      <c r="E77" s="14" t="s">
+      <c r="D78" s="14"/>
+      <c r="E78" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B78" s="15" t="s">
+    <row r="79" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B79" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C78" s="15">
+      <c r="C79" s="15">
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B79" s="25" t="s">
+    <row r="80" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B80" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C79" s="25"/>
-      <c r="D79" s="25"/>
-      <c r="E79" s="25"/>
-    </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B80" s="16"/>
-      <c r="C80" s="6" t="s">
+      <c r="C80" s="37"/>
+      <c r="D80" s="37"/>
+      <c r="E80" s="37"/>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B81" s="16"/>
+      <c r="C81" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D80" s="6" t="s">
+      <c r="D81" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E80" s="6" t="s">
+      <c r="E81" s="6" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B81" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C81" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D81" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E81" s="9" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B82" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C82" s="9"/>
-      <c r="D82" s="9"/>
-      <c r="E82" s="9"/>
+        <v>25</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D82" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B83" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C83" s="9" t="s">
-        <v>17</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C83" s="9"/>
       <c r="D83" s="9"/>
       <c r="E83" s="9"/>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B84" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D84" s="9"/>
       <c r="E84" s="9"/>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B85" s="17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D85" s="9"/>
       <c r="E85" s="9"/>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B86" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C86" s="18"/>
-      <c r="D86" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E86" s="9" t="s">
-        <v>27</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B87" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C87" s="18"/>
+        <v>74</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>75</v>
+      </c>
       <c r="D87" s="9"/>
       <c r="E87" s="9"/>
+      <c r="F87" s="14"/>
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B88" s="25" t="s">
+      <c r="B88" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C88" s="18"/>
+      <c r="D88" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B89" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C89" s="18"/>
+      <c r="D89" s="9"/>
+      <c r="E89" s="9"/>
+    </row>
+    <row r="90" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B90" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="C88" s="25"/>
-      <c r="D88" s="25"/>
-    </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B89" s="6" t="s">
+      <c r="C90" s="37"/>
+      <c r="D90" s="37"/>
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B91" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C89" s="6" t="s">
+      <c r="C91" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D89" s="6" t="s">
+      <c r="D91" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E89" s="6" t="s">
+      <c r="E91" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F89" s="26" t="s">
+      <c r="F91" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="G89" s="27"/>
-      <c r="H89" s="27"/>
-      <c r="I89" s="27"/>
-      <c r="J89" s="27"/>
-      <c r="K89" s="28"/>
-    </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B90" s="9" t="s">
+      <c r="G91" s="29"/>
+      <c r="H91" s="29"/>
+      <c r="I91" s="29"/>
+      <c r="J91" s="29"/>
+      <c r="K91" s="30"/>
+    </row>
+    <row r="92" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B92" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C90" s="9" t="s">
+      <c r="C92" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D90" s="9"/>
-      <c r="E90" s="9"/>
-      <c r="F90" s="29"/>
-      <c r="G90" s="30"/>
-      <c r="H90" s="30"/>
-      <c r="I90" s="30"/>
-      <c r="J90" s="30"/>
-      <c r="K90" s="31"/>
-    </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B91" s="9" t="s">
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="25"/>
+      <c r="G92" s="26"/>
+      <c r="H92" s="26"/>
+      <c r="I92" s="26"/>
+      <c r="J92" s="26"/>
+      <c r="K92" s="27"/>
+    </row>
+    <row r="93" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B93" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C91" s="9" t="s">
+      <c r="C93" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D91" s="9"/>
-      <c r="E91" s="9"/>
-      <c r="F91" s="32" t="s">
+      <c r="D93" s="9"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="G91" s="33"/>
-      <c r="H91" s="33"/>
-      <c r="I91" s="33"/>
-      <c r="J91" s="33"/>
-      <c r="K91" s="34"/>
-    </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B92" s="17" t="s">
+      <c r="G93" s="32"/>
+      <c r="H93" s="32"/>
+      <c r="I93" s="32"/>
+      <c r="J93" s="32"/>
+      <c r="K93" s="33"/>
+    </row>
+    <row r="94" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B94" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C92" s="9">
+      <c r="C94" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B93" s="17" t="s">
+    <row r="95" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B95" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C93" s="9">
+      <c r="C95" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B95" s="5" t="s">
+    <row r="97" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B97" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C95" s="5" t="s">
+      <c r="C97" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D95" s="14"/>
-      <c r="E95" s="14" t="s">
+      <c r="D97" s="14"/>
+      <c r="E97" s="14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="96" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B96" s="15" t="s">
+    <row r="98" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B98" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C96" s="15">
+      <c r="C98" s="15">
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B97" s="25" t="s">
+    <row r="99" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B99" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C97" s="25"/>
-      <c r="D97" s="25"/>
-      <c r="E97" s="25"/>
-    </row>
-    <row r="98" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B98" s="16"/>
-      <c r="C98" s="6" t="s">
+      <c r="C99" s="37"/>
+      <c r="D99" s="37"/>
+      <c r="E99" s="37"/>
+    </row>
+    <row r="100" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B100" s="16"/>
+      <c r="C100" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D98" s="6" t="s">
+      <c r="D100" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E98" s="6" t="s">
+      <c r="E100" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="99" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B99" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C99" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="D99" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E99" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="100" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B100" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C100" s="9"/>
-      <c r="D100" s="9"/>
-      <c r="E100" s="9"/>
     </row>
     <row r="101" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B101" s="17" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D101" s="9"/>
-      <c r="E101" s="9"/>
+        <v>51</v>
+      </c>
+      <c r="D101" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="102" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B102" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C102" s="9" t="s">
-        <v>54</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C102" s="9"/>
       <c r="D102" s="9"/>
       <c r="E102" s="9"/>
     </row>
-    <row r="103" spans="2:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B103" s="17" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D103" s="9"/>
       <c r="E103" s="9"/>
     </row>
     <row r="104" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B104" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C104" s="18"/>
-      <c r="D104" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E104" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="105" spans="2:11" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="C104" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D104" s="9"/>
+      <c r="E104" s="9"/>
+    </row>
+    <row r="105" spans="2:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B105" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C105" s="18"/>
+        <v>35</v>
+      </c>
+      <c r="C105" s="9" t="s">
+        <v>36</v>
+      </c>
       <c r="D105" s="9"/>
       <c r="E105" s="9"/>
     </row>
-    <row r="106" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B106" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C106" s="25"/>
-      <c r="D106" s="25"/>
+    <row r="106" spans="2:11" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B106" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C106" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D106" s="9"/>
+      <c r="E106" s="9"/>
     </row>
     <row r="107" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B107" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C107" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D107" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E107" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F107" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="G107" s="27"/>
-      <c r="H107" s="27"/>
-      <c r="I107" s="27"/>
-      <c r="J107" s="27"/>
-      <c r="K107" s="28"/>
+      <c r="B107" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C107" s="18"/>
+      <c r="D107" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E107" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="108" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B108" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C108" s="9" t="s">
-        <v>44</v>
-      </c>
+      <c r="B108" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C108" s="18"/>
       <c r="D108" s="9"/>
       <c r="E108" s="9"/>
-      <c r="F108" s="29"/>
-      <c r="G108" s="30"/>
-      <c r="H108" s="30"/>
-      <c r="I108" s="30"/>
-      <c r="J108" s="30"/>
-      <c r="K108" s="31"/>
-    </row>
-    <row r="109" spans="2:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B109" s="24" t="s">
+    </row>
+    <row r="109" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B109" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C109" s="37"/>
+      <c r="D109" s="37"/>
+    </row>
+    <row r="110" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B110" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C110" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E110" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F110" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="G110" s="29"/>
+      <c r="H110" s="29"/>
+      <c r="I110" s="29"/>
+      <c r="J110" s="29"/>
+      <c r="K110" s="30"/>
+    </row>
+    <row r="111" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B111" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C111" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D111" s="9"/>
+      <c r="E111" s="9"/>
+      <c r="F111" s="25"/>
+      <c r="G111" s="26"/>
+      <c r="H111" s="26"/>
+      <c r="I111" s="26"/>
+      <c r="J111" s="26"/>
+      <c r="K111" s="27"/>
+    </row>
+    <row r="112" spans="2:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B112" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="C109" s="24" t="s">
+      <c r="C112" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D109" s="24"/>
-      <c r="E109" s="24"/>
-      <c r="F109" s="35" t="s">
+      <c r="D112" s="24"/>
+      <c r="E112" s="24"/>
+      <c r="F112" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="G109" s="36"/>
-      <c r="H109" s="36"/>
-      <c r="I109" s="36"/>
-      <c r="J109" s="36"/>
-      <c r="K109" s="37"/>
-    </row>
-    <row r="110" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B110" s="17" t="s">
+      <c r="G112" s="35"/>
+      <c r="H112" s="35"/>
+      <c r="I112" s="35"/>
+      <c r="J112" s="35"/>
+      <c r="K112" s="36"/>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B113" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C110" s="9">
+      <c r="C113" s="9">
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B111" s="17" t="s">
+    <row r="114" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B114" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C111" s="9">
+      <c r="C114" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B113" s="5" t="s">
+    <row r="116" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B116" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C113" s="5" t="s">
+      <c r="C116" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D113" s="14"/>
-      <c r="E113" s="14" t="s">
+      <c r="D116" s="14"/>
+      <c r="E116" s="14" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="114" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B114" s="15" t="s">
+    <row r="117" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B117" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C114" s="15" t="s">
+      <c r="C117" s="15" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="115" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B115" s="25" t="s">
+    <row r="118" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B118" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C115" s="25"/>
-      <c r="D115" s="25"/>
-      <c r="E115" s="25"/>
-    </row>
-    <row r="116" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B116" s="16"/>
-      <c r="C116" s="6" t="s">
+      <c r="C118" s="37"/>
+      <c r="D118" s="37"/>
+      <c r="E118" s="37"/>
+    </row>
+    <row r="119" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B119" s="16"/>
+      <c r="C119" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D116" s="6" t="s">
+      <c r="D119" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E116" s="6" t="s">
+      <c r="E119" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="117" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B117" s="17" t="s">
+    <row r="120" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B120" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C117" s="9" t="s">
+      <c r="C120" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D117" s="9" t="s">
+      <c r="D120" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E117" s="9" t="s">
+      <c r="E120" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="118" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B118" s="17" t="s">
+    <row r="121" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B121" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C118" s="9"/>
-      <c r="D118" s="9"/>
-      <c r="E118" s="9"/>
-    </row>
-    <row r="119" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B119" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C119" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D119" s="9"/>
-      <c r="E119" s="9"/>
-    </row>
-    <row r="120" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B120" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C120" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D120" s="9"/>
-      <c r="E120" s="9"/>
-    </row>
-    <row r="121" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B121" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C121" s="9" t="s">
-        <v>36</v>
-      </c>
+      <c r="C121" s="9"/>
       <c r="D121" s="9"/>
       <c r="E121" s="9"/>
     </row>
-    <row r="122" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B122" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C122" s="18"/>
-      <c r="D122" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E122" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="123" spans="2:11" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="C122" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D122" s="9"/>
+      <c r="E122" s="9"/>
+    </row>
+    <row r="123" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B123" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C123" s="18"/>
+        <v>32</v>
+      </c>
+      <c r="C123" s="9" t="s">
+        <v>55</v>
+      </c>
       <c r="D123" s="9"/>
       <c r="E123" s="9"/>
     </row>
-    <row r="124" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B124" s="25" t="s">
+    <row r="124" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B124" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C124" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D124" s="9"/>
+      <c r="E124" s="9"/>
+    </row>
+    <row r="125" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B125" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C125" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D125" s="9"/>
+      <c r="E125" s="9"/>
+    </row>
+    <row r="126" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B126" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C126" s="18"/>
+      <c r="D126" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E126" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B127" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C127" s="18"/>
+      <c r="D127" s="9"/>
+      <c r="E127" s="9"/>
+    </row>
+    <row r="128" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B128" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="C124" s="25"/>
-      <c r="D124" s="25"/>
-    </row>
-    <row r="125" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B125" s="6" t="s">
+      <c r="C128" s="37"/>
+      <c r="D128" s="37"/>
+    </row>
+    <row r="129" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B129" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C125" s="6" t="s">
+      <c r="C129" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D125" s="6" t="s">
+      <c r="D129" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E125" s="6" t="s">
+      <c r="E129" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F125" s="26" t="s">
+      <c r="F129" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="G125" s="27"/>
-      <c r="H125" s="27"/>
-      <c r="I125" s="27"/>
-      <c r="J125" s="27"/>
-      <c r="K125" s="28"/>
-    </row>
-    <row r="126" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B126" s="9" t="s">
+      <c r="G129" s="29"/>
+      <c r="H129" s="29"/>
+      <c r="I129" s="29"/>
+      <c r="J129" s="29"/>
+      <c r="K129" s="30"/>
+    </row>
+    <row r="130" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B130" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C126" s="9" t="s">
+      <c r="C130" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D126" s="9"/>
-      <c r="E126" s="9"/>
-      <c r="F126" s="29"/>
-      <c r="G126" s="30"/>
-      <c r="H126" s="30"/>
-      <c r="I126" s="30"/>
-      <c r="J126" s="30"/>
-      <c r="K126" s="31"/>
-    </row>
-    <row r="127" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B127" s="17" t="s">
+      <c r="D130" s="9"/>
+      <c r="E130" s="9"/>
+      <c r="F130" s="25"/>
+      <c r="G130" s="26"/>
+      <c r="H130" s="26"/>
+      <c r="I130" s="26"/>
+      <c r="J130" s="26"/>
+      <c r="K130" s="27"/>
+    </row>
+    <row r="131" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B131" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C127" s="9">
+      <c r="C131" s="9">
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B128" s="17" t="s">
+    <row r="132" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B132" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C128" s="9">
+      <c r="C132" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B130" s="5" t="s">
+    <row r="134" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B134" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C130" s="5" t="s">
+      <c r="C134" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D130" s="14"/>
-      <c r="E130" s="14" t="s">
+      <c r="D134" s="14"/>
+      <c r="E134" s="14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="131" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B131" s="15" t="s">
+    <row r="135" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B135" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C131" s="15" t="s">
+      <c r="C135" s="15" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="132" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B132" s="25" t="s">
+    <row r="136" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B136" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C132" s="25"/>
-      <c r="D132" s="25"/>
-      <c r="E132" s="25"/>
-    </row>
-    <row r="133" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B133" s="16"/>
-      <c r="C133" s="6" t="s">
+      <c r="C136" s="37"/>
+      <c r="D136" s="37"/>
+      <c r="E136" s="37"/>
+    </row>
+    <row r="137" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B137" s="16"/>
+      <c r="C137" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D133" s="6" t="s">
+      <c r="D137" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E133" s="6" t="s">
+      <c r="E137" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="134" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B134" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C134" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D134" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E134" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="135" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B135" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C135" s="9"/>
-      <c r="D135" s="9"/>
-      <c r="E135" s="9"/>
-    </row>
-    <row r="136" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B136" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C136" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D136" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E136" s="9"/>
-    </row>
-    <row r="137" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B137" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C137" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D137" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E137" s="9"/>
     </row>
     <row r="138" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B138" s="17" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C138" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D138" s="9"/>
-      <c r="E138" s="9"/>
+        <v>52</v>
+      </c>
+      <c r="D138" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E138" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="139" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B139" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C139" s="18"/>
-      <c r="D139" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="E139" s="9" t="s">
-        <v>27</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C139" s="9"/>
+      <c r="D139" s="9"/>
+      <c r="E139" s="9"/>
     </row>
     <row r="140" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B140" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C140" s="18"/>
-      <c r="D140" s="9"/>
+        <v>31</v>
+      </c>
+      <c r="C140" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D140" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="E140" s="9"/>
     </row>
     <row r="141" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B141" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C141" s="25"/>
-      <c r="D141" s="25"/>
+      <c r="B141" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C141" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D141" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E141" s="9"/>
     </row>
     <row r="142" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B142" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C142" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D142" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E142" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F142" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="G142" s="27"/>
-      <c r="H142" s="27"/>
-      <c r="I142" s="27"/>
-      <c r="J142" s="27"/>
-      <c r="K142" s="28"/>
+      <c r="B142" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C142" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D142" s="9"/>
+      <c r="E142" s="9"/>
     </row>
     <row r="143" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B143" s="9" t="s">
-        <v>10</v>
+      <c r="B143" s="17" t="s">
+        <v>74</v>
       </c>
       <c r="C143" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D143" s="9" t="s">
-        <v>72</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="D143" s="9"/>
       <c r="E143" s="9"/>
-      <c r="F143" s="29"/>
-      <c r="G143" s="30"/>
-      <c r="H143" s="30"/>
-      <c r="I143" s="30"/>
-      <c r="J143" s="30"/>
-      <c r="K143" s="31"/>
     </row>
     <row r="144" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B144" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C144" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D144" s="9"/>
-      <c r="E144" s="9"/>
-      <c r="F144" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="G144" s="33"/>
-      <c r="H144" s="33"/>
-      <c r="I144" s="33"/>
-      <c r="J144" s="33"/>
-      <c r="K144" s="34"/>
+      <c r="B144" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C144" s="18"/>
+      <c r="D144" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E144" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="145" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B145" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C145" s="18"/>
+      <c r="D145" s="9"/>
+      <c r="E145" s="9"/>
+    </row>
+    <row r="146" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B146" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C146" s="37"/>
+      <c r="D146" s="37"/>
+    </row>
+    <row r="147" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B147" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C147" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D147" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E147" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F147" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="G147" s="29"/>
+      <c r="H147" s="29"/>
+      <c r="I147" s="29"/>
+      <c r="J147" s="29"/>
+      <c r="K147" s="30"/>
+    </row>
+    <row r="148" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B148" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C148" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D148" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E148" s="9"/>
+      <c r="F148" s="25"/>
+      <c r="G148" s="26"/>
+      <c r="H148" s="26"/>
+      <c r="I148" s="26"/>
+      <c r="J148" s="26"/>
+      <c r="K148" s="27"/>
+    </row>
+    <row r="149" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B149" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C149" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D149" s="9"/>
+      <c r="E149" s="9"/>
+      <c r="F149" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="G149" s="32"/>
+      <c r="H149" s="32"/>
+      <c r="I149" s="32"/>
+      <c r="J149" s="32"/>
+      <c r="K149" s="33"/>
+    </row>
+    <row r="150" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B150" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C145" s="9">
+      <c r="C150" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B146" s="17" t="s">
+    <row r="151" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B151" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C146" s="9">
+      <c r="C151" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="148" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B148" s="22" t="s">
+    <row r="153" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B153" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C148" s="22" t="s">
+      <c r="C153" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D148" s="14"/>
-      <c r="E148" s="14" t="s">
+      <c r="D153" s="14"/>
+      <c r="E153" s="14" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="149" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B149" s="15" t="s">
+    <row r="154" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B154" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C149" s="15">
+      <c r="C154" s="15">
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B150" s="25" t="s">
+    <row r="155" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B155" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C150" s="25"/>
-      <c r="D150" s="25"/>
-      <c r="E150" s="25"/>
-    </row>
-    <row r="151" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B151" s="16"/>
-      <c r="C151" s="6" t="s">
+      <c r="C155" s="37"/>
+      <c r="D155" s="37"/>
+      <c r="E155" s="37"/>
+    </row>
+    <row r="156" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B156" s="16"/>
+      <c r="C156" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D151" s="6" t="s">
+      <c r="D156" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E151" s="6" t="s">
+      <c r="E156" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="152" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B152" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C152" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D152" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E152" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="153" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B153" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C153" s="9"/>
-      <c r="D153" s="9"/>
-      <c r="E153" s="9"/>
-    </row>
-    <row r="154" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B154" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C154" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D154" s="9"/>
-      <c r="E154" s="9"/>
-    </row>
-    <row r="155" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B155" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C155" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D155" s="9"/>
-      <c r="E155" s="9"/>
-    </row>
-    <row r="156" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B156" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C156" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D156" s="9"/>
-      <c r="E156" s="9"/>
     </row>
     <row r="157" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B157" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C157" s="18"/>
+        <v>25</v>
+      </c>
+      <c r="C157" s="9" t="s">
+        <v>52</v>
+      </c>
       <c r="D157" s="9" t="s">
         <v>53</v>
       </c>
@@ -2133,283 +2145,353 @@
     </row>
     <row r="158" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B158" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C158" s="18"/>
+        <v>30</v>
+      </c>
+      <c r="C158" s="9"/>
       <c r="D158" s="9"/>
       <c r="E158" s="9"/>
     </row>
     <row r="159" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B159" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C159" s="25"/>
-      <c r="D159" s="25"/>
+      <c r="B159" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C159" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D159" s="9"/>
+      <c r="E159" s="9"/>
     </row>
     <row r="160" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B160" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C160" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D160" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E160" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F160" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="G160" s="27"/>
-      <c r="H160" s="27"/>
-      <c r="I160" s="27"/>
-      <c r="J160" s="27"/>
-      <c r="K160" s="28"/>
+      <c r="B160" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C160" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D160" s="9"/>
+      <c r="E160" s="9"/>
     </row>
     <row r="161" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B161" s="9" t="s">
-        <v>10</v>
+      <c r="B161" s="17" t="s">
+        <v>35</v>
       </c>
       <c r="C161" s="9" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D161" s="9"/>
       <c r="E161" s="9"/>
-      <c r="F161" s="29"/>
-      <c r="G161" s="30"/>
-      <c r="H161" s="30"/>
-      <c r="I161" s="30"/>
-      <c r="J161" s="30"/>
-      <c r="K161" s="31"/>
     </row>
     <row r="162" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B162" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C162" s="9">
-        <v>3</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="C162" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D162" s="9"/>
+      <c r="E162" s="9"/>
     </row>
     <row r="163" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B163" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C163" s="9">
-        <v>1</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C163" s="18"/>
+      <c r="D163" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E163" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="164" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B164" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C164" s="18"/>
+      <c r="D164" s="9"/>
+      <c r="E164" s="9"/>
     </row>
     <row r="165" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B165" s="23" t="s">
+      <c r="B165" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C165" s="37"/>
+      <c r="D165" s="37"/>
+    </row>
+    <row r="166" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B166" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C166" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C165" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D165" s="14"/>
-      <c r="E165" s="14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="166" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B166" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="C166" s="15" t="s">
-        <v>50</v>
-      </c>
+      <c r="D166" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E166" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F166" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="G166" s="29"/>
+      <c r="H166" s="29"/>
+      <c r="I166" s="29"/>
+      <c r="J166" s="29"/>
+      <c r="K166" s="30"/>
     </row>
     <row r="167" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B167" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C167" s="25"/>
-      <c r="D167" s="25"/>
-      <c r="E167" s="25"/>
+      <c r="B167" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C167" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D167" s="9"/>
+      <c r="E167" s="9"/>
+      <c r="F167" s="25"/>
+      <c r="G167" s="26"/>
+      <c r="H167" s="26"/>
+      <c r="I167" s="26"/>
+      <c r="J167" s="26"/>
+      <c r="K167" s="27"/>
     </row>
     <row r="168" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B168" s="16"/>
-      <c r="C168" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D168" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E168" s="6" t="s">
-        <v>24</v>
+      <c r="B168" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C168" s="9">
+        <v>3</v>
       </c>
     </row>
     <row r="169" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B169" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C169" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D169" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E169" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="170" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B170" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="C170" s="9"/>
-      <c r="D170" s="9"/>
-      <c r="E170" s="9"/>
+        <v>47</v>
+      </c>
+      <c r="C169" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="171" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B171" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C171" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D171" s="9"/>
-      <c r="E171" s="9"/>
+      <c r="B171" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C171" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D171" s="14"/>
+      <c r="E171" s="14" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="172" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B172" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C172" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D172" s="9"/>
-      <c r="E172" s="9"/>
+      <c r="B172" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C172" s="15" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="173" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B173" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C173" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D173" s="9"/>
-      <c r="E173" s="9"/>
+      <c r="B173" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="C173" s="37"/>
+      <c r="D173" s="37"/>
+      <c r="E173" s="37"/>
     </row>
     <row r="174" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B174" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C174" s="18"/>
-      <c r="D174" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E174" s="9" t="s">
-        <v>27</v>
+      <c r="B174" s="16"/>
+      <c r="C174" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D174" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E174" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="175" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B175" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C175" s="18"/>
-      <c r="D175" s="9"/>
-      <c r="E175" s="9"/>
+        <v>25</v>
+      </c>
+      <c r="C175" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D175" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E175" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="176" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B176" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C176" s="25"/>
-      <c r="D176" s="25"/>
+      <c r="B176" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C176" s="9"/>
+      <c r="D176" s="9"/>
+      <c r="E176" s="9"/>
     </row>
     <row r="177" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B177" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C177" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D177" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E177" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F177" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="G177" s="27"/>
-      <c r="H177" s="27"/>
-      <c r="I177" s="27"/>
-      <c r="J177" s="27"/>
-      <c r="K177" s="28"/>
+      <c r="B177" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C177" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D177" s="9"/>
+      <c r="E177" s="9"/>
     </row>
     <row r="178" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B178" s="9" t="s">
-        <v>10</v>
+      <c r="B178" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="C178" s="9" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D178" s="9"/>
       <c r="E178" s="9"/>
-      <c r="F178" s="29"/>
-      <c r="G178" s="30"/>
-      <c r="H178" s="30"/>
-      <c r="I178" s="30"/>
-      <c r="J178" s="30"/>
-      <c r="K178" s="31"/>
     </row>
     <row r="179" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B179" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C179" s="9">
-        <v>3</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C179" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D179" s="9"/>
+      <c r="E179" s="9"/>
     </row>
     <row r="180" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B180" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C180" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D180" s="9"/>
+      <c r="E180" s="9"/>
+    </row>
+    <row r="181" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B181" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C181" s="18"/>
+      <c r="D181" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E181" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="182" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B182" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C182" s="18"/>
+      <c r="D182" s="9"/>
+      <c r="E182" s="9"/>
+    </row>
+    <row r="183" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B183" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C183" s="37"/>
+      <c r="D183" s="37"/>
+    </row>
+    <row r="184" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B184" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C184" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D184" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E184" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F184" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="G184" s="29"/>
+      <c r="H184" s="29"/>
+      <c r="I184" s="29"/>
+      <c r="J184" s="29"/>
+      <c r="K184" s="30"/>
+    </row>
+    <row r="185" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B185" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C185" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D185" s="9"/>
+      <c r="E185" s="9"/>
+      <c r="F185" s="25"/>
+      <c r="G185" s="26"/>
+      <c r="H185" s="26"/>
+      <c r="I185" s="26"/>
+      <c r="J185" s="26"/>
+      <c r="K185" s="27"/>
+    </row>
+    <row r="186" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B186" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C186" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="187" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B187" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C180" s="9">
+      <c r="C187" s="9">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="34">
-    <mergeCell ref="F90:K90"/>
-    <mergeCell ref="F107:K107"/>
-    <mergeCell ref="F108:K108"/>
-    <mergeCell ref="F125:K125"/>
-    <mergeCell ref="F126:K126"/>
-    <mergeCell ref="F91:K91"/>
-    <mergeCell ref="F109:K109"/>
-    <mergeCell ref="B106:D106"/>
-    <mergeCell ref="B124:D124"/>
-    <mergeCell ref="B167:E167"/>
+    <mergeCell ref="B183:D183"/>
+    <mergeCell ref="F184:K184"/>
+    <mergeCell ref="F185:K185"/>
+    <mergeCell ref="B146:D146"/>
+    <mergeCell ref="B118:E118"/>
+    <mergeCell ref="F147:K147"/>
+    <mergeCell ref="F148:K148"/>
+    <mergeCell ref="B136:E136"/>
+    <mergeCell ref="F166:K166"/>
+    <mergeCell ref="F167:K167"/>
+    <mergeCell ref="F149:K149"/>
+    <mergeCell ref="B109:D109"/>
+    <mergeCell ref="B128:D128"/>
+    <mergeCell ref="B173:E173"/>
     <mergeCell ref="G2:K2"/>
     <mergeCell ref="B61:E61"/>
-    <mergeCell ref="B79:E79"/>
-    <mergeCell ref="B70:D70"/>
-    <mergeCell ref="B88:D88"/>
-    <mergeCell ref="B97:E97"/>
+    <mergeCell ref="B80:E80"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B90:D90"/>
+    <mergeCell ref="B99:E99"/>
     <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B150:E150"/>
-    <mergeCell ref="B159:D159"/>
-    <mergeCell ref="F71:K71"/>
+    <mergeCell ref="B155:E155"/>
+    <mergeCell ref="B165:D165"/>
     <mergeCell ref="F72:K72"/>
     <mergeCell ref="F73:K73"/>
-    <mergeCell ref="F89:K89"/>
-    <mergeCell ref="B176:D176"/>
-    <mergeCell ref="F177:K177"/>
-    <mergeCell ref="F178:K178"/>
-    <mergeCell ref="B141:D141"/>
-    <mergeCell ref="B115:E115"/>
-    <mergeCell ref="F142:K142"/>
-    <mergeCell ref="F143:K143"/>
-    <mergeCell ref="B132:E132"/>
-    <mergeCell ref="F160:K160"/>
-    <mergeCell ref="F161:K161"/>
-    <mergeCell ref="F144:K144"/>
+    <mergeCell ref="F74:K74"/>
+    <mergeCell ref="F91:K91"/>
+    <mergeCell ref="F92:K92"/>
+    <mergeCell ref="F110:K110"/>
+    <mergeCell ref="F111:K111"/>
+    <mergeCell ref="F129:K129"/>
+    <mergeCell ref="F130:K130"/>
+    <mergeCell ref="F93:K93"/>
+    <mergeCell ref="F112:K112"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2421,9 +2503,9 @@
   <rowBreaks count="5" manualBreakCount="5">
     <brk id="18" max="11" man="1"/>
     <brk id="57" max="16383" man="1"/>
-    <brk id="94" max="11" man="1"/>
-    <brk id="129" max="11" man="1"/>
-    <brk id="164" max="11" man="1"/>
+    <brk id="96" max="11" man="1"/>
+    <brk id="133" max="11" man="1"/>
+    <brk id="170" max="11" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -2436,6 +2518,9 @@
     <sheetView topLeftCell="A60" workbookViewId="0">
       <selection sqref="A1:A86"/>
     </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="1">
+      <selection sqref="A1:A87"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2469,13 +2554,13 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B60&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C60&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D60&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E59&amp;CHAR(34)&amp;"&gt;"</f>
-        <v xml:space="preserve">  &lt;schedule scheduleName="P1" dose="1" indication="BIRTH" label="2 months"&gt;</v>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B60&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C60&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D60&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E59&amp;CHAR(34)&amp;" indicationEnd="&amp;CHAR(34)&amp;Schedules!C68&amp;CHAR(34)&amp;"&gt;"</f>
+        <v xml:space="preserve">  &lt;schedule scheduleName="P1" dose="1" indication="BIRTH" label="2 months" indicationEnd="19 years"&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C75&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C74&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C76&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C75&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="1"/&gt;</v>
       </c>
     </row>
@@ -2511,25 +2596,25 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D68&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E68&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D69&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E69&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="0 days" grace=""/&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D69&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D70&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B72&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C72&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D72&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F72&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E72&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B73&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C73&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D73&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F73&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E73&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="PCV" schedule="P2" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B73&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C73&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D73&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F73&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E73&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B74&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C74&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D74&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F74&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E74&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="12 Months Old" schedule="C2" age="" reason="First valid dose not received by 12 months of age, only 2 doses needed now." historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
@@ -2541,67 +2626,67 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B78&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C78&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D78&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E77&amp;CHAR(34)&amp;"&gt;"</f>
-        <v xml:space="preserve">  &lt;schedule scheduleName="P2" dose="2" indication="" label="4 months"&gt;</v>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B79&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C79&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D79&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E78&amp;CHAR(34)&amp;" indicationEnd="&amp;CHAR(34)&amp;Schedules!C87&amp;CHAR(34)&amp;"&gt;"</f>
+        <v xml:space="preserve">  &lt;schedule scheduleName="P2" dose="2" indication="" label="4 months" indicationEnd="19 years"&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C93&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C92&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C95&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C94&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="2"/&gt;</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C81&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D81&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E81&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C82&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D82&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E82&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="10 weeks" interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C82&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D82&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E82&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C83&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D83&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E83&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C83&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D83&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E83&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C84&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D84&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E84&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="4 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C84&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D84&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E84&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C85&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D85&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E85&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="5 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C85&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D85&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E85&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C86&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D86&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E86&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="5 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D86&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E86&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D88&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E88&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D87&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D89&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="21" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B90&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C90&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D90&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F90&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E90&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B92&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C92&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D92&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F92&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E92&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="PCV" schedule="P3" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B91&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C91&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D91&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F91&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E91&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B93&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C93&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D93&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F93&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E93&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="12 Months Old" schedule="C2" age="" reason="Second valid dose was not received by 12 months of age, only 2 more doses needed now." historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
@@ -2613,67 +2698,67 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B96&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C96&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D96&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E95&amp;CHAR(34)&amp;"&gt;"</f>
-        <v xml:space="preserve">  &lt;schedule scheduleName="P3" dose="3" indication="" label="6 months"&gt;</v>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B98&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C98&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D98&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E97&amp;CHAR(34)&amp;" indicationEnd="&amp;CHAR(34)&amp;Schedules!C106&amp;CHAR(34)&amp;"&gt;"</f>
+        <v xml:space="preserve">  &lt;schedule scheduleName="P3" dose="3" indication="" label="6 months" indicationEnd="19 years"&gt;</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C111&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C110&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C114&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C113&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="3"/&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C99&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D99&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E99&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C101&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D101&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E101&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="14 weeks" interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C100&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D100&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E100&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C102&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D102&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E102&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C101&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D101&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E101&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C103&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D103&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E103&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="6 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C102&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D102&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E102&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C104&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D104&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E104&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="7 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C103&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D103&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E103&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C105&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D105&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E105&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="5 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D104&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E104&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D107&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E107&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="20" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D105&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D108&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="21" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B108&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C108&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D108&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F108&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E108&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B111&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C111&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D111&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F111&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E111&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="PCV" schedule="P4" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="21" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B109&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C109&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D109&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F109&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E109&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B112&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C112&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D112&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F112&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E112&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="12 Months Old" schedule="C3" age="" reason="Third valid dose was not received by 12 months of age, the third and final dose should be given as soon as possible." historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
@@ -2685,61 +2770,61 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B114&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C114&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D114&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E113&amp;CHAR(34)&amp;"&gt;"</f>
-        <v xml:space="preserve">  &lt;schedule scheduleName="P4" dose="B" indication="" label="booster"&gt;</v>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B117&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C117&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D117&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E116&amp;CHAR(34)&amp;" indicationEnd="&amp;CHAR(34)&amp;Schedules!C125&amp;CHAR(34)&amp;"&gt;"</f>
+        <v xml:space="preserve">  &lt;schedule scheduleName="P4" dose="B" indication="" label="booster" indicationEnd="19 years"&gt;</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C128&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C127&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C132&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C131&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="1" column="4"/&gt;</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="20" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C117&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D117&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E117&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C120&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D120&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E120&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="12 months" interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="20" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C118&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D118&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E118&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C121&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D121&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E121&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="20" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C119&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D119&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E119&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C122&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D122&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E122&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="12 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="20" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C120&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D120&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E120&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C123&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D123&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E123&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="16 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="20" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C121&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D121&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E121&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C124&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D124&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E124&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="5 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="20" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D122&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E122&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D126&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E126&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D123&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D127&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="21" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B126&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C126&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D126&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F126&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E126&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B130&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C130&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D130&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F130&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E130&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="PCV" schedule="COMPLETE" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
@@ -2751,67 +2836,67 @@
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="20" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B131&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C131&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D131&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E130&amp;CHAR(34)&amp;"&gt;"</f>
-        <v xml:space="preserve">  &lt;schedule scheduleName="C2" dose="*" indication="" label="2nd dose 12 month catchup"&gt;</v>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B135&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C135&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D135&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E134&amp;CHAR(34)&amp;" indicationEnd="&amp;CHAR(34)&amp;Schedules!C143&amp;CHAR(34)&amp;"&gt;"</f>
+        <v xml:space="preserve">  &lt;schedule scheduleName="C2" dose="*" indication="" label="2nd dose 12 month catchup" indicationEnd="19 years"&gt;</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="19" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C146&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C145&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C151&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C150&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="2" column="2"/&gt;</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="20" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C134&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D134&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E134&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C138&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D138&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E138&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="12 months" interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="20" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C135&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D135&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E135&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C139&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D139&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E139&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="20" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C136&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D136&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E136&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C140&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D140&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E140&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="12 months" interval="4 weeks" grace=""/&gt;</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="20" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C137&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D137&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E137&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C141&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D141&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E141&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="12 months" interval="4 weeks" grace=""/&gt;</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="20" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C138&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D138&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E138&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C142&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D142&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E142&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="5 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="20" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D139&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E139&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D144&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E144&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="4 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" s="20" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D140&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D145&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="21" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B143&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C143&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D143&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F143&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E143&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B148&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C148&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D148&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F148&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E148&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="PCV" schedule="C4" age="24 months -4 d" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" s="21" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B144&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C144&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D144&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F144&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E144&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B149&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C149&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D149&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F149&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E149&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="PCV" schedule="COMPLETE" age="" reason="Second valid dose received after 24 months of age, no more doses needed." historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
@@ -2823,61 +2908,61 @@
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" s="20" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B149&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C149&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D149&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E148&amp;CHAR(34)&amp;"&gt;"</f>
-        <v xml:space="preserve">  &lt;schedule scheduleName="C3" dose="3" indication="" label="3rd dose 12 month catchup"&gt;</v>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B154&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C154&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D154&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E153&amp;CHAR(34)&amp;" indicationEnd="&amp;CHAR(34)&amp;Schedules!C162&amp;CHAR(34)&amp;"&gt;"</f>
+        <v xml:space="preserve">  &lt;schedule scheduleName="C3" dose="3" indication="" label="3rd dose 12 month catchup" indicationEnd="19 years"&gt;</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="19" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C164&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C163&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C170&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C169&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="" column="1"/&gt;</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" s="20" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C152&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D152&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E152&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C157&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D157&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E157&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="12 months" interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" s="20" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C153&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D153&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E153&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C158&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D158&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E158&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" s="20" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C154&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D154&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E154&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C159&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D159&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E159&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="12 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="20" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C155&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D155&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E155&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C160&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D160&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E160&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="12 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" s="20" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C156&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D156&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E156&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C161&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D161&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E161&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="5 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" s="20" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D157&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E157&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D163&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E163&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" s="20" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D158&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D164&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" s="21" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B161&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C161&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D161&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F161&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E161&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B167&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C167&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D167&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F167&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E167&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="PCV" schedule="COMPLETE" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>
@@ -2889,61 +2974,61 @@
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" s="20" t="str">
-        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B166&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C166&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D166&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E165&amp;CHAR(34)&amp;"&gt;"</f>
-        <v xml:space="preserve">  &lt;schedule scheduleName="C4" dose="B" indication="" label="booster"&gt;</v>
+        <f>"  &lt;schedule scheduleName="&amp;CHAR(34)&amp;Schedules!B172&amp;CHAR(34)&amp;" dose="&amp;CHAR(34)&amp;Schedules!C172&amp;CHAR(34)&amp;" indication="&amp;CHAR(34)&amp;Schedules!D172&amp;CHAR(34)&amp;" label="&amp;CHAR(34)&amp;Schedules!E171&amp;CHAR(34)&amp;" indicationEnd="&amp;CHAR(34)&amp;Schedules!C180&amp;CHAR(34)&amp;"&gt;"</f>
+        <v xml:space="preserve">  &lt;schedule scheduleName="C4" dose="B" indication="" label="booster" indicationEnd="19 years"&gt;</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" s="19" t="str">
-        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C181&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C180&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;pos row="&amp;CHAR(34)&amp;Schedules!C188&amp;CHAR(34)&amp;" column="&amp;CHAR(34)&amp;Schedules!C187&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;pos row="" column="3"/&gt;</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" s="20" t="str">
-        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C169&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D169&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E169&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;valid age="&amp;CHAR(34)&amp;Schedules!C175&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D175&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E175&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;valid age="12 months" interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" s="20" t="str">
-        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C170&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D170&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E170&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;early age="&amp;CHAR(34)&amp;Schedules!C176&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D176&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E176&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;early age="" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" s="20" t="str">
-        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C171&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D171&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E171&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;due age="&amp;CHAR(34)&amp;Schedules!C177&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D177&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E177&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;due age="12 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" s="20" t="str">
-        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C172&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D172&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E172&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;overdue age="&amp;CHAR(34)&amp;Schedules!C178&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D178&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E178&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;overdue age="12 months" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" s="20" t="str">
-        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C173&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D173&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E173&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;finished age="&amp;CHAR(34)&amp;Schedules!C179&amp;CHAR(34)&amp;" interval="&amp;CHAR(34)&amp;Schedules!D179&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E179&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;finished age="5 years" interval="" grace=""/&gt;</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" s="20" t="str">
-        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D174&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E174&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;after-invalid interval="&amp;CHAR(34)&amp;Schedules!D181&amp;CHAR(34)&amp;" grace="&amp;CHAR(34)&amp;Schedules!E181&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;after-invalid interval="8 weeks" grace="4 days"/&gt;</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" s="20" t="str">
-        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D175&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;before-previous interval="&amp;CHAR(34)&amp;Schedules!D182&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;before-previous interval=""/&gt;</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" s="21" t="str">
-        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B178&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C178&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D178&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F178&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E178&amp;CHAR(34)&amp;"/&gt;"</f>
+        <f>"    &lt;indicate vaccineName="&amp;CHAR(34)&amp;Schedules!B185&amp;CHAR(34)&amp;" schedule="&amp;CHAR(34)&amp;Schedules!C185&amp;CHAR(34)&amp;" age="&amp;CHAR(34)&amp;Schedules!D185&amp;CHAR(34)&amp;" reason="&amp;CHAR(34)&amp;Schedules!F185&amp;CHAR(34)&amp;" historyOfVaccineName="&amp;CHAR(34)&amp;Schedules!E185&amp;CHAR(34)&amp;"/&gt;"</f>
         <v xml:space="preserve">    &lt;indicate vaccineName="PCV" schedule="COMPLETE" age="" reason="" historyOfVaccineName=""/&gt;</v>
       </c>
     </row>

</xml_diff>